<commit_message>
introduce dcterms mapping, annotations from values  and new iris of individuals
</commit_message>
<xml_diff>
--- a/tests/csv_pipeline_test/input/mapping/tensile_test_mapping.xlsx
+++ b/tests/csv_pipeline_test/input/mapping/tensile_test_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Key</t>
   </si>
@@ -31,55 +31,52 @@
     <t>TestingFacility</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Projektnummer</t>
   </si>
   <si>
-    <t>ProjectNumber</t>
+    <t>https://w3id.org/steel/ProcessOntology/ProjectNumber</t>
   </si>
   <si>
     <t>Projektname</t>
   </si>
   <si>
-    <t>ProjectName</t>
+    <t>https://w3id.org/steel/ProcessOntology/ProjectName</t>
   </si>
   <si>
     <t>Datum/Uhrzeit</t>
   </si>
   <si>
-    <t>TimeStamp</t>
+    <t>https://w3id.org/steel/ProcessOntology/TimeStamp</t>
   </si>
   <si>
     <t>Maschinendaten</t>
   </si>
   <si>
-    <t>MachineData</t>
+    <t>https://w3id.org/steel/ProcessOntology/MachineData</t>
   </si>
   <si>
     <t>Kraftaufnehmer</t>
   </si>
   <si>
-    <t>ForceMeasuringDevice</t>
+    <t>https://w3id.org/steel/ProcessOntology/ForceMeasuringDevice</t>
   </si>
   <si>
     <t>Wegaufnehmer</t>
   </si>
   <si>
-    <t>DisplacementTransducer</t>
+    <t>https://w3id.org/steel/ProcessOntology/DisplacementTransducer</t>
   </si>
   <si>
     <t>Prüfnorm</t>
   </si>
   <si>
-    <t>TestStandard</t>
+    <t>https://w3id.org/steel/ProcessOntology/TestStandard</t>
   </si>
   <si>
     <t>Werkstoff</t>
   </si>
   <si>
-    <t>Material</t>
+    <t>https://w3id.org/steel/ProcessOntology/Material</t>
   </si>
   <si>
     <t>https://w3id.org/steel/ProcessOntology</t>
@@ -88,103 +85,103 @@
     <t>Probentyp</t>
   </si>
   <si>
-    <t>SpecimenType</t>
+    <t>https://w3id.org/steel/ProcessOntology/SpecimenType</t>
   </si>
   <si>
     <t>Prüfer</t>
   </si>
   <si>
-    <t>Tester</t>
+    <t>https://w3id.org/steel/ProcessOntology/Tester</t>
   </si>
   <si>
     <t>Probenkennung 2</t>
   </si>
   <si>
-    <t>SampleIdentifier-2</t>
+    <t>https://w3id.org/steel/ProcessOntology/SampleIdentifier-2</t>
   </si>
   <si>
     <t>Messlänge Standardweg</t>
   </si>
   <si>
-    <t>OriginalGaugeLength</t>
+    <t>https://w3id.org/steel/ProcessOntology/OriginalGaugeLength</t>
   </si>
   <si>
     <t>Versuchslänge</t>
   </si>
   <si>
-    <t>ParallelLength</t>
+    <t>https://w3id.org/steel/ProcessOntology/ParallelLength</t>
   </si>
   <si>
     <t>Probendicke</t>
   </si>
   <si>
-    <t>SpecimenThickness</t>
+    <t>https://w3id.org/steel/ProcessOntology/SpecimenThickness</t>
   </si>
   <si>
     <t>Probenbreite</t>
   </si>
   <si>
-    <t>SpecimenWidth</t>
+    <t>https://w3id.org/steel/ProcessOntology/SpecimenWidth</t>
   </si>
   <si>
     <t>Prüfgeschwindigkeit</t>
   </si>
   <si>
-    <t>TestingRate</t>
+    <t>https://w3id.org/steel/ProcessOntology/TestingRate</t>
   </si>
   <si>
     <t>Vorkraft</t>
   </si>
   <si>
-    <t>Preload</t>
+    <t>https://w3id.org/steel/ProcessOntology/Preload</t>
   </si>
   <si>
     <t>Temperatur</t>
   </si>
   <si>
-    <t>Temperature</t>
+    <t>https://w3id.org/steel/ProcessOntology/Temperature</t>
   </si>
   <si>
     <t>Bemerkung</t>
   </si>
   <si>
-    <t>Remark</t>
+    <t>https://w3id.org/steel/ProcessOntology/Remark</t>
   </si>
   <si>
     <t>Prüfzeit</t>
   </si>
   <si>
-    <t>TestTime</t>
+    <t>https://w3id.org/steel/ProcessOntology/TestTime</t>
   </si>
   <si>
     <t>Standardkraft</t>
   </si>
   <si>
-    <t>StandardForce</t>
+    <t>https://w3id.org/steel/ProcessOntology/StandardForce</t>
   </si>
   <si>
     <t>Traversenweg absolut</t>
   </si>
   <si>
-    <t>AbsoluteCrossheadTravel</t>
+    <t>https://w3id.org/steel/ProcessOntology/AbsoluteCrossheadTravel</t>
   </si>
   <si>
     <t>Standardweg</t>
   </si>
   <si>
-    <t>Extension</t>
+    <t>https://w3id.org/steel/ProcessOntology/Extension</t>
   </si>
   <si>
     <t>Breitenänderung</t>
   </si>
   <si>
-    <t>WidthChange</t>
+    <t>https://w3id.org/steel/ProcessOntology/WidthChange</t>
   </si>
   <si>
     <t>Dehnung</t>
   </si>
   <si>
-    <t>PercentageElongation</t>
+    <t>https://w3id.org/steel/ProcessOntology/PercentageElongation</t>
   </si>
 </sst>
 </file>
@@ -202,7 +199,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -242,15 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -564,9 +558,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="62.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="64.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -580,296 +574,244 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C24" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C27" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>

</xml_diff>

<commit_message>
entirely restructure parsers and mappings
</commit_message>
<xml_diff>
--- a/tests/csv_pipeline_test/input/mapping/tensile_test_mapping.xlsx
+++ b/tests/csv_pipeline_test/input/mapping/tensile_test_mapping.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Class type</t>
-  </si>
-  <si>
-    <t>Annotation</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>iri</t>
+  </si>
+  <si>
+    <t>annotation</t>
   </si>
   <si>
     <t>Prüfinstitut</t>
@@ -563,7 +563,7 @@
     <col min="3" max="3" style="3" width="64.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>